<commit_message>
amend document yesterdays work
</commit_message>
<xml_diff>
--- a/Arbeitsverlauf/Dokumentation Arbeitsverlauf Janina Hosch.xlsx
+++ b/Arbeitsverlauf/Dokumentation Arbeitsverlauf Janina Hosch.xlsx
@@ -3,24 +3,32 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220E22BD-E536-46D1-B1F3-9B247903653A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB974285-CC7F-4C49-A2BD-FF186C21FD37}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Mo, 02.03.2020" sheetId="6" r:id="rId1"/>
+    <sheet name="Mo, 02.03.2020" sheetId="8" r:id="rId1"/>
+    <sheet name="Di, 03.03.2020" sheetId="6" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>1.</t>
   </si>
@@ -70,7 +78,16 @@
     <t>Lernfeld</t>
   </si>
   <si>
-    <t>-</t>
+    <t>alle</t>
+  </si>
+  <si>
+    <t>Einarbeitung in das bereits bestehende Projekt: Requirements, Projektstruktur, Architektur</t>
+  </si>
+  <si>
+    <t>Pflichtenheft</t>
+  </si>
+  <si>
+    <t>Pflichtenheft-Struktur besteht, einige Anforderungen sind bereits beschrieben</t>
   </si>
 </sst>
 </file>
@@ -114,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -132,6 +149,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -412,11 +435,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3BF081-D2C7-4C42-897B-02772E17735A}">
-  <dimension ref="B1:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4531F262-D706-4BDF-A55A-3ACA28D63712}">
+  <dimension ref="B1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,65 +474,225 @@
       <c r="D2" s="6"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C3" s="4">
+    <row r="3" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="8">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="3"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="9" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="13" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="17" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
+      <c r="D14" s="6"/>
+    </row>
+    <row r="18" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="21" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
+      <c r="D18" s="6"/>
+    </row>
+    <row r="22" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="6"/>
+      <c r="D22" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3BF081-D2C7-4C42-897B-02772E17735A}">
+  <dimension ref="B1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="101.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="71.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="8">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C4" s="9"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D11" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="18" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="22" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEFB9E8-A7F4-4F02-8C82-B96E445D7B85}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>